<commit_message>
Update rounding for pip calculation
</commit_message>
<xml_diff>
--- a/edge_research/dataout/18dpip.xlsx
+++ b/edge_research/dataout/18dpip.xlsx
@@ -412,7 +412,7 @@
         <v>43102</v>
       </c>
       <c r="B2">
-        <v>27.99999999999914</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1.35494</v>
@@ -426,7 +426,7 @@
         <v>43103</v>
       </c>
       <c r="B3">
-        <v>13.90000000000002</v>
+        <v>13.9</v>
       </c>
       <c r="C3">
         <v>1.34995</v>
@@ -440,7 +440,7 @@
         <v>43104</v>
       </c>
       <c r="B4">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C4">
         <v>1.35534</v>
@@ -454,7 +454,7 @@
         <v>43105</v>
       </c>
       <c r="B5">
-        <v>0.700000000000145</v>
+        <v>0.7</v>
       </c>
       <c r="C5">
         <v>1.35622</v>
@@ -468,7 +468,7 @@
         <v>43108</v>
       </c>
       <c r="B6">
-        <v>25.90000000000092</v>
+        <v>25.9</v>
       </c>
       <c r="C6">
         <v>1.35537</v>
@@ -482,7 +482,7 @@
         <v>43109</v>
       </c>
       <c r="B7">
-        <v>5.299999999999194</v>
+        <v>5.3</v>
       </c>
       <c r="C7">
         <v>1.35157</v>
@@ -496,7 +496,7 @@
         <v>43110</v>
       </c>
       <c r="B8">
-        <v>-3.60000000000138</v>
+        <v>-3.6</v>
       </c>
       <c r="C8">
         <v>1.35315</v>
@@ -510,7 +510,7 @@
         <v>43111</v>
       </c>
       <c r="B9">
-        <v>4.500000000000615</v>
+        <v>4.5</v>
       </c>
       <c r="C9">
         <v>1.35334</v>
@@ -524,7 +524,7 @@
         <v>43112</v>
       </c>
       <c r="B10">
-        <v>12.19999999999999</v>
+        <v>12.2</v>
       </c>
       <c r="C10">
         <v>1.36733</v>
@@ -538,7 +538,7 @@
         <v>43115</v>
       </c>
       <c r="B11">
-        <v>19.19999999999922</v>
+        <v>19.2</v>
       </c>
       <c r="C11">
         <v>1.37839</v>
@@ -552,7 +552,7 @@
         <v>43116</v>
       </c>
       <c r="B12">
-        <v>9.500000000000064</v>
+        <v>9.5</v>
       </c>
       <c r="C12">
         <v>1.37637</v>
@@ -566,7 +566,7 @@
         <v>43117</v>
       </c>
       <c r="B13">
-        <v>29.09999999999746</v>
+        <v>29.1</v>
       </c>
       <c r="C13">
         <v>1.38047</v>
@@ -580,7 +580,7 @@
         <v>43118</v>
       </c>
       <c r="B14">
-        <v>7.399999999999629</v>
+        <v>7.4</v>
       </c>
       <c r="C14">
         <v>1.38751</v>
@@ -594,7 +594,7 @@
         <v>43119</v>
       </c>
       <c r="B15">
-        <v>-14.70000000000082</v>
+        <v>-14.7</v>
       </c>
       <c r="C15">
         <v>1.3864</v>
@@ -608,7 +608,7 @@
         <v>43122</v>
       </c>
       <c r="B16">
-        <v>26.19999999999845</v>
+        <v>26.2</v>
       </c>
       <c r="C16">
         <v>1.39386</v>
@@ -622,7 +622,7 @@
         <v>43123</v>
       </c>
       <c r="B17">
-        <v>-0.5999999999972694</v>
+        <v>-0.6</v>
       </c>
       <c r="C17">
         <v>1.40138</v>
@@ -636,7 +636,7 @@
         <v>43124</v>
       </c>
       <c r="B18">
-        <v>10.30000000000086</v>
+        <v>10.3</v>
       </c>
       <c r="C18">
         <v>1.42149</v>
@@ -650,7 +650,7 @@
         <v>43125</v>
       </c>
       <c r="B19">
-        <v>4.199999999998649</v>
+        <v>4.2</v>
       </c>
       <c r="C19">
         <v>1.43019</v>
@@ -664,7 +664,7 @@
         <v>43126</v>
       </c>
       <c r="B20">
-        <v>24.60000000000129</v>
+        <v>24.6</v>
       </c>
       <c r="C20">
         <v>1.41631</v>
@@ -678,7 +678,7 @@
         <v>43129</v>
       </c>
       <c r="B21">
-        <v>-23.6000000000014</v>
+        <v>-23.6</v>
       </c>
       <c r="C21">
         <v>1.40836</v>
@@ -692,7 +692,7 @@
         <v>43130</v>
       </c>
       <c r="B22">
-        <v>-6.299999999999084</v>
+        <v>-6.3</v>
       </c>
       <c r="C22">
         <v>1.41265</v>
@@ -706,7 +706,7 @@
         <v>43131</v>
       </c>
       <c r="B23">
-        <v>32.99999999999859</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1.41962</v>
@@ -720,7 +720,7 @@
         <v>43132</v>
       </c>
       <c r="B24">
-        <v>14.10000000000133</v>
+        <v>14.1</v>
       </c>
       <c r="C24">
         <v>1.42203</v>
@@ -734,7 +734,7 @@
         <v>43133</v>
       </c>
       <c r="B25">
-        <v>-2.900000000001235</v>
+        <v>-2.9</v>
       </c>
       <c r="C25">
         <v>1.41291</v>
@@ -748,7 +748,7 @@
         <v>43136</v>
       </c>
       <c r="B26">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C26">
         <v>1.40236</v>
@@ -762,7 +762,7 @@
         <v>43137</v>
       </c>
       <c r="B27">
-        <v>53.19999999999769</v>
+        <v>53.2</v>
       </c>
       <c r="C27">
         <v>1.38596</v>
@@ -776,7 +776,7 @@
         <v>43138</v>
       </c>
       <c r="B28">
-        <v>-23.40000000000231</v>
+        <v>-23.4</v>
       </c>
       <c r="C28">
         <v>1.39057</v>
@@ -790,7 +790,7 @@
         <v>43139</v>
       </c>
       <c r="B29">
-        <v>-17.60000000000206</v>
+        <v>-17.6</v>
       </c>
       <c r="C29">
         <v>1.40125</v>
@@ -804,7 +804,7 @@
         <v>43140</v>
       </c>
       <c r="B30">
-        <v>9.200000000000319</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="C30">
         <v>1.3801</v>
@@ -818,7 +818,7 @@
         <v>43143</v>
       </c>
       <c r="B31">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C31">
         <v>1.38067</v>
@@ -832,7 +832,7 @@
         <v>43144</v>
       </c>
       <c r="B32">
-        <v>-15.40000000000097</v>
+        <v>-15.4</v>
       </c>
       <c r="C32">
         <v>1.38937</v>
@@ -846,7 +846,7 @@
         <v>43145</v>
       </c>
       <c r="B33">
-        <v>68.79999999999997</v>
+        <v>68.8</v>
       </c>
       <c r="C33">
         <v>1.38952</v>
@@ -860,7 +860,7 @@
         <v>43146</v>
       </c>
       <c r="B34">
-        <v>-5.300000000001415</v>
+        <v>-5.3</v>
       </c>
       <c r="C34">
         <v>1.40657</v>
@@ -874,7 +874,7 @@
         <v>43147</v>
       </c>
       <c r="B35">
-        <v>-3.199999999998759</v>
+        <v>-3.2</v>
       </c>
       <c r="C35">
         <v>1.40462</v>
@@ -888,7 +888,7 @@
         <v>43150</v>
       </c>
       <c r="B36">
-        <v>9.099999999999664</v>
+        <v>9.1</v>
       </c>
       <c r="C36">
         <v>1.39815</v>
@@ -902,7 +902,7 @@
         <v>43151</v>
       </c>
       <c r="B37">
-        <v>18.19999999999933</v>
+        <v>18.2</v>
       </c>
       <c r="C37">
         <v>1.39886</v>
@@ -916,7 +916,7 @@
         <v>43152</v>
       </c>
       <c r="B38">
-        <v>9.200000000000319</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="C38">
         <v>1.39713</v>
@@ -930,7 +930,7 @@
         <v>43153</v>
       </c>
       <c r="B39">
-        <v>-1.699999999997814</v>
+        <v>-1.7</v>
       </c>
       <c r="C39">
         <v>1.39413</v>
@@ -944,7 +944,7 @@
         <v>43154</v>
       </c>
       <c r="B40">
-        <v>-18.69999999999816</v>
+        <v>-18.7</v>
       </c>
       <c r="C40">
         <v>1.39908</v>
@@ -958,7 +958,7 @@
         <v>43157</v>
       </c>
       <c r="B41">
-        <v>-11.39999999999919</v>
+        <v>-11.4</v>
       </c>
       <c r="C41">
         <v>1.39488</v>
@@ -972,7 +972,7 @@
         <v>43158</v>
       </c>
       <c r="B42">
-        <v>-24.60000000000129</v>
+        <v>-24.6</v>
       </c>
       <c r="C42">
         <v>1.3904</v>
@@ -986,7 +986,7 @@
         <v>43159</v>
       </c>
       <c r="B43">
-        <v>-14.09999999999911</v>
+        <v>-14.1</v>
       </c>
       <c r="C43">
         <v>1.37919</v>
@@ -1000,7 +1000,7 @@
         <v>43160</v>
       </c>
       <c r="B44">
-        <v>-6.799999999997919</v>
+        <v>-6.8</v>
       </c>
       <c r="C44">
         <v>1.37298</v>
@@ -1014,7 +1014,7 @@
         <v>43161</v>
       </c>
       <c r="B45">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C45">
         <v>1.37769</v>
@@ -1028,7 +1028,7 @@
         <v>43164</v>
       </c>
       <c r="B46">
-        <v>29.69999999999695</v>
+        <v>29.7</v>
       </c>
       <c r="C46">
         <v>1.38146</v>
@@ -1042,7 +1042,7 @@
         <v>43165</v>
       </c>
       <c r="B47">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C47">
         <v>1.38924</v>
@@ -1056,7 +1056,7 @@
         <v>43166</v>
       </c>
       <c r="B48">
-        <v>23.89999999999892</v>
+        <v>23.9</v>
       </c>
       <c r="C48">
         <v>1.387</v>
@@ -1070,7 +1070,7 @@
         <v>43167</v>
       </c>
       <c r="B49">
-        <v>-25.10000000000012</v>
+        <v>-25.1</v>
       </c>
       <c r="C49">
         <v>1.38587</v>
@@ -1084,7 +1084,7 @@
         <v>43168</v>
       </c>
       <c r="B50">
-        <v>-12.50000000000195</v>
+        <v>-12.5</v>
       </c>
       <c r="C50">
         <v>1.38778</v>
@@ -1098,7 +1098,7 @@
         <v>43171</v>
       </c>
       <c r="B51">
-        <v>15.19999999999966</v>
+        <v>15.2</v>
       </c>
       <c r="C51">
         <v>1.38809</v>
@@ -1112,7 +1112,7 @@
         <v>43172</v>
       </c>
       <c r="B52">
-        <v>14.89999999999991</v>
+        <v>14.9</v>
       </c>
       <c r="C52">
         <v>1.39521</v>
@@ -1126,7 +1126,7 @@
         <v>43173</v>
       </c>
       <c r="B53">
-        <v>3.80000000000047</v>
+        <v>3.8</v>
       </c>
       <c r="C53">
         <v>1.3959</v>
@@ -1140,7 +1140,7 @@
         <v>43174</v>
       </c>
       <c r="B54">
-        <v>11.79999999999959</v>
+        <v>11.8</v>
       </c>
       <c r="C54">
         <v>1.39707</v>
@@ -1154,7 +1154,7 @@
         <v>43175</v>
       </c>
       <c r="B55">
-        <v>-28.00000000000136</v>
+        <v>-28</v>
       </c>
       <c r="C55">
         <v>1.39282</v>
@@ -1168,7 +1168,7 @@
         <v>43178</v>
       </c>
       <c r="B56">
-        <v>-11.79999999999959</v>
+        <v>-11.8</v>
       </c>
       <c r="C56">
         <v>1.4045</v>
@@ -1182,7 +1182,7 @@
         <v>43179</v>
       </c>
       <c r="B57">
-        <v>9.899999999998244</v>
+        <v>9.9</v>
       </c>
       <c r="C57">
         <v>1.39942</v>
@@ -1196,7 +1196,7 @@
         <v>43180</v>
       </c>
       <c r="B58">
-        <v>-1.399999999998069</v>
+        <v>-1.4</v>
       </c>
       <c r="C58">
         <v>1.40705</v>
@@ -1210,7 +1210,7 @@
         <v>43181</v>
       </c>
       <c r="B59">
-        <v>-13.60000000000028</v>
+        <v>-13.6</v>
       </c>
       <c r="C59">
         <v>1.41157</v>
@@ -1224,7 +1224,7 @@
         <v>43182</v>
       </c>
       <c r="B60">
-        <v>1.40000000000029</v>
+        <v>1.4</v>
       </c>
       <c r="C60">
         <v>1.41601</v>
@@ -1238,7 +1238,7 @@
         <v>43185</v>
       </c>
       <c r="B61">
-        <v>22.8000000000006</v>
+        <v>22.8</v>
       </c>
       <c r="C61">
         <v>1.41991</v>
@@ -1252,7 +1252,7 @@
         <v>43186</v>
       </c>
       <c r="B62">
-        <v>-6.599999999996609</v>
+        <v>-6.6</v>
       </c>
       <c r="C62">
         <v>1.41473</v>
@@ -1266,7 +1266,7 @@
         <v>43187</v>
       </c>
       <c r="B63">
-        <v>7.200000000000539</v>
+        <v>7.2</v>
       </c>
       <c r="C63">
         <v>1.40955</v>
@@ -1280,7 +1280,7 @@
         <v>43188</v>
       </c>
       <c r="B64">
-        <v>-44.49999999999843</v>
+        <v>-44.5</v>
       </c>
       <c r="C64">
         <v>1.40672</v>
@@ -1294,7 +1294,7 @@
         <v>43189</v>
       </c>
       <c r="B65">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C65">
         <v>1.40365</v>
@@ -1308,7 +1308,7 @@
         <v>43192</v>
       </c>
       <c r="B66">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C66">
         <v>1.40542</v>
@@ -1322,7 +1322,7 @@
         <v>43193</v>
       </c>
       <c r="B67">
-        <v>5.199999999998539</v>
+        <v>5.2</v>
       </c>
       <c r="C67">
         <v>1.40366</v>
@@ -1336,7 +1336,7 @@
         <v>43194</v>
       </c>
       <c r="B68">
-        <v>-3.999999999999559</v>
+        <v>-4</v>
       </c>
       <c r="C68">
         <v>1.40841</v>
@@ -1350,7 +1350,7 @@
         <v>43195</v>
       </c>
       <c r="B69">
-        <v>-16.10000000000111</v>
+        <v>-16.1</v>
       </c>
       <c r="C69">
         <v>1.40145</v>
@@ -1364,7 +1364,7 @@
         <v>43196</v>
       </c>
       <c r="B70">
-        <v>-8.400000000001739</v>
+        <v>-8.4</v>
       </c>
       <c r="C70">
         <v>1.40935</v>
@@ -1378,7 +1378,7 @@
         <v>43199</v>
       </c>
       <c r="B71">
-        <v>-15.39999999999875</v>
+        <v>-15.4</v>
       </c>
       <c r="C71">
         <v>1.4142</v>
@@ -1392,7 +1392,7 @@
         <v>43200</v>
       </c>
       <c r="B72">
-        <v>-5.299999999999194</v>
+        <v>-5.3</v>
       </c>
       <c r="C72">
         <v>1.41759</v>
@@ -1406,7 +1406,7 @@
         <v>43201</v>
       </c>
       <c r="B73">
-        <v>-1.500000000000945</v>
+        <v>-1.5</v>
       </c>
       <c r="C73">
         <v>1.42048</v>
@@ -1420,7 +1420,7 @@
         <v>43202</v>
       </c>
       <c r="B74">
-        <v>23.40000000000009</v>
+        <v>23.4</v>
       </c>
       <c r="C74">
         <v>1.42076</v>
@@ -1434,7 +1434,7 @@
         <v>43203</v>
       </c>
       <c r="B75">
-        <v>-8.500000000000174</v>
+        <v>-8.5</v>
       </c>
       <c r="C75">
         <v>1.42528</v>
@@ -1448,7 +1448,7 @@
         <v>43206</v>
       </c>
       <c r="B76">
-        <v>13.19999999999988</v>
+        <v>13.2</v>
       </c>
       <c r="C76">
         <v>1.43187</v>
@@ -1462,7 +1462,7 @@
         <v>43207</v>
       </c>
       <c r="B77">
-        <v>-1.899999999999125</v>
+        <v>-1.9</v>
       </c>
       <c r="C77">
         <v>1.43095</v>
@@ -1476,7 +1476,7 @@
         <v>43208</v>
       </c>
       <c r="B78">
-        <v>0.700000000000145</v>
+        <v>0.7</v>
       </c>
       <c r="C78">
         <v>1.42303</v>
@@ -1490,7 +1490,7 @@
         <v>43209</v>
       </c>
       <c r="B79">
-        <v>-9.500000000000064</v>
+        <v>-9.5</v>
       </c>
       <c r="C79">
         <v>1.42317</v>
@@ -1504,7 +1504,7 @@
         <v>43210</v>
       </c>
       <c r="B80">
-        <v>3.999999999999559</v>
+        <v>4</v>
       </c>
       <c r="C80">
         <v>1.40203</v>
@@ -1518,7 +1518,7 @@
         <v>43213</v>
       </c>
       <c r="B81">
-        <v>-8.199999999998209</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="C81">
         <v>1.39549</v>
@@ -1532,7 +1532,7 @@
         <v>43214</v>
       </c>
       <c r="B82">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C82">
         <v>1.39644</v>
@@ -1546,7 +1546,7 @@
         <v>43215</v>
       </c>
       <c r="B83">
-        <v>6.300000000001305</v>
+        <v>6.3</v>
       </c>
       <c r="C83">
         <v>1.39298</v>
@@ -1560,7 +1560,7 @@
         <v>43216</v>
       </c>
       <c r="B84">
-        <v>-28.90000000000059</v>
+        <v>-28.9</v>
       </c>
       <c r="C84">
         <v>1.39552</v>
@@ -1574,7 +1574,7 @@
         <v>43217</v>
       </c>
       <c r="B85">
-        <v>18.70000000000038</v>
+        <v>18.7</v>
       </c>
       <c r="C85">
         <v>1.37781</v>
@@ -1588,7 +1588,7 @@
         <v>43220</v>
       </c>
       <c r="B86">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C86">
         <v>1.37687</v>
@@ -1602,7 +1602,7 @@
         <v>43221</v>
       </c>
       <c r="B87">
-        <v>-30.59999999999841</v>
+        <v>-30.6</v>
       </c>
       <c r="C87">
         <v>1.36233</v>
@@ -1616,7 +1616,7 @@
         <v>43222</v>
       </c>
       <c r="B88">
-        <v>-18.49999999999907</v>
+        <v>-18.5</v>
       </c>
       <c r="C88">
         <v>1.36123</v>
@@ -1630,7 +1630,7 @@
         <v>43223</v>
       </c>
       <c r="B89">
-        <v>-32.30000000000067</v>
+        <v>-32.3</v>
       </c>
       <c r="C89">
         <v>1.35772</v>
@@ -1644,7 +1644,7 @@
         <v>43224</v>
       </c>
       <c r="B90">
-        <v>4.700000000001925</v>
+        <v>4.7</v>
       </c>
       <c r="C90">
         <v>1.35118</v>
@@ -1658,7 +1658,7 @@
         <v>43227</v>
       </c>
       <c r="B91">
-        <v>8.400000000001739</v>
+        <v>8.4</v>
       </c>
       <c r="C91">
         <v>1.35613</v>
@@ -1672,7 +1672,7 @@
         <v>43228</v>
       </c>
       <c r="B92">
-        <v>28.40000000000176</v>
+        <v>28.4</v>
       </c>
       <c r="C92">
         <v>1.34875</v>
@@ -1686,7 +1686,7 @@
         <v>43229</v>
       </c>
       <c r="B93">
-        <v>2.699999999999925</v>
+        <v>2.7</v>
       </c>
       <c r="C93">
         <v>1.35762</v>
@@ -1700,7 +1700,7 @@
         <v>43230</v>
       </c>
       <c r="B94">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C94">
         <v>1.34723</v>
@@ -1714,7 +1714,7 @@
         <v>43231</v>
       </c>
       <c r="B95">
-        <v>-16.30000000000242</v>
+        <v>-16.3</v>
       </c>
       <c r="C95">
         <v>1.35671</v>
@@ -1728,7 +1728,7 @@
         <v>43234</v>
       </c>
       <c r="B96">
-        <v>6.399999999999739</v>
+        <v>6.4</v>
       </c>
       <c r="C96">
         <v>1.35872</v>
@@ -1742,7 +1742,7 @@
         <v>43235</v>
       </c>
       <c r="B97">
-        <v>15.79999999999915</v>
+        <v>15.8</v>
       </c>
       <c r="C97">
         <v>1.34777</v>
@@ -1756,7 +1756,7 @@
         <v>43236</v>
       </c>
       <c r="B98">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C98">
         <v>1.34873</v>
@@ -1770,7 +1770,7 @@
         <v>43237</v>
       </c>
       <c r="B99">
-        <v>-6.699999999997264</v>
+        <v>-6.7</v>
       </c>
       <c r="C99">
         <v>1.35044</v>
@@ -1784,7 +1784,7 @@
         <v>43238</v>
       </c>
       <c r="B100">
-        <v>4.399999999999959</v>
+        <v>4.4</v>
       </c>
       <c r="C100">
         <v>1.34704</v>
@@ -1798,7 +1798,7 @@
         <v>43241</v>
       </c>
       <c r="B101">
-        <v>-9.100000000001884</v>
+        <v>-9.1</v>
       </c>
       <c r="C101">
         <v>1.34147</v>
@@ -1812,7 +1812,7 @@
         <v>43242</v>
       </c>
       <c r="B102">
-        <v>-16.40000000000308</v>
+        <v>-16.4</v>
       </c>
       <c r="C102">
         <v>1.34367</v>
@@ -1826,7 +1826,7 @@
         <v>43243</v>
       </c>
       <c r="B103">
-        <v>-16.19999999999955</v>
+        <v>-16.2</v>
       </c>
       <c r="C103">
         <v>1.33571</v>
@@ -1840,7 +1840,7 @@
         <v>43244</v>
       </c>
       <c r="B104">
-        <v>-16.89999999999969</v>
+        <v>-16.9</v>
       </c>
       <c r="C104">
         <v>1.33878</v>
@@ -1854,7 +1854,7 @@
         <v>43245</v>
       </c>
       <c r="B105">
-        <v>2.499999999998614</v>
+        <v>2.5</v>
       </c>
       <c r="C105">
         <v>1.33136</v>
@@ -1868,7 +1868,7 @@
         <v>43248</v>
       </c>
       <c r="B106">
-        <v>-5.100000000000104</v>
+        <v>-5.1</v>
       </c>
       <c r="C106">
         <v>1.33045</v>
@@ -1882,7 +1882,7 @@
         <v>43249</v>
       </c>
       <c r="B107">
-        <v>-14.00000000000068</v>
+        <v>-14</v>
       </c>
       <c r="C107">
         <v>1.32822</v>
@@ -1896,7 +1896,7 @@
         <v>43250</v>
       </c>
       <c r="B108">
-        <v>-10.19999999999799</v>
+        <v>-10.2</v>
       </c>
       <c r="C108">
         <v>1.32829</v>
@@ -1910,7 +1910,7 @@
         <v>43251</v>
       </c>
       <c r="B109">
-        <v>-21.50000000000096</v>
+        <v>-21.5</v>
       </c>
       <c r="C109">
         <v>1.3321</v>
@@ -1924,7 +1924,7 @@
         <v>43252</v>
       </c>
       <c r="B110">
-        <v>4.20000000000087</v>
+        <v>4.2</v>
       </c>
       <c r="C110">
         <v>1.33238</v>
@@ -1938,7 +1938,7 @@
         <v>43255</v>
       </c>
       <c r="B111">
-        <v>-21.40000000000253</v>
+        <v>-21.4</v>
       </c>
       <c r="C111">
         <v>1.33537</v>
@@ -1952,7 +1952,7 @@
         <v>43256</v>
       </c>
       <c r="B112">
-        <v>7.500000000000284</v>
+        <v>7.5</v>
       </c>
       <c r="C112">
         <v>1.33361</v>
@@ -1966,7 +1966,7 @@
         <v>43257</v>
       </c>
       <c r="B113">
-        <v>-2.19999999999887</v>
+        <v>-2.2</v>
       </c>
       <c r="C113">
         <v>1.34273</v>
@@ -1980,7 +1980,7 @@
         <v>43258</v>
       </c>
       <c r="B114">
-        <v>31.5999999999983</v>
+        <v>31.6</v>
       </c>
       <c r="C114">
         <v>1.33897</v>
@@ -1994,7 +1994,7 @@
         <v>43259</v>
       </c>
       <c r="B115">
-        <v>18.19999999999933</v>
+        <v>18.2</v>
       </c>
       <c r="C115">
         <v>1.33881</v>
@@ -2008,7 +2008,7 @@
         <v>43262</v>
       </c>
       <c r="B116">
-        <v>-3.599999999999159</v>
+        <v>-3.6</v>
       </c>
       <c r="C116">
         <v>1.33961</v>
@@ -2022,7 +2022,7 @@
         <v>43263</v>
       </c>
       <c r="B117">
-        <v>-10.59999999999839</v>
+        <v>-10.6</v>
       </c>
       <c r="C117">
         <v>1.33638</v>
@@ -2036,7 +2036,7 @@
         <v>43264</v>
       </c>
       <c r="B118">
-        <v>5.699999999999594</v>
+        <v>5.7</v>
       </c>
       <c r="C118">
         <v>1.33609</v>
@@ -2050,7 +2050,7 @@
         <v>43265</v>
       </c>
       <c r="B119">
-        <v>16.7000000000006</v>
+        <v>16.7</v>
       </c>
       <c r="C119">
         <v>1.33153</v>
@@ -2064,7 +2064,7 @@
         <v>43266</v>
       </c>
       <c r="B120">
-        <v>5.60000000000116</v>
+        <v>5.6</v>
       </c>
       <c r="C120">
         <v>1.32755</v>
@@ -2078,7 +2078,7 @@
         <v>43269</v>
       </c>
       <c r="B121">
-        <v>2.8000000000028</v>
+        <v>2.8</v>
       </c>
       <c r="C121">
         <v>1.32393</v>
@@ -2092,7 +2092,7 @@
         <v>43270</v>
       </c>
       <c r="B122">
-        <v>7.600000000000939</v>
+        <v>7.6</v>
       </c>
       <c r="C122">
         <v>1.31609</v>
@@ -2106,7 +2106,7 @@
         <v>43271</v>
       </c>
       <c r="B123">
-        <v>1.19999999999898</v>
+        <v>1.2</v>
       </c>
       <c r="C123">
         <v>1.3176</v>
@@ -2120,7 +2120,7 @@
         <v>43272</v>
       </c>
       <c r="B124">
-        <v>9.399999999999409</v>
+        <v>9.4</v>
       </c>
       <c r="C124">
         <v>1.32491</v>
@@ -2134,7 +2134,7 @@
         <v>43273</v>
       </c>
       <c r="B125">
-        <v>14.40000000000108</v>
+        <v>14.4</v>
       </c>
       <c r="C125">
         <v>1.32552</v>
@@ -2148,7 +2148,7 @@
         <v>43276</v>
       </c>
       <c r="B126">
-        <v>-5.899999999998684</v>
+        <v>-5.9</v>
       </c>
       <c r="C126">
         <v>1.3272</v>
@@ -2162,7 +2162,7 @@
         <v>43277</v>
       </c>
       <c r="B127">
-        <v>2.99999999999967</v>
+        <v>3</v>
       </c>
       <c r="C127">
         <v>1.32305</v>
@@ -2176,7 +2176,7 @@
         <v>43278</v>
       </c>
       <c r="B128">
-        <v>-8.799999999999919</v>
+        <v>-8.800000000000001</v>
       </c>
       <c r="C128">
         <v>1.31552</v>
@@ -2190,7 +2190,7 @@
         <v>43279</v>
       </c>
       <c r="B129">
-        <v>-8.500000000000174</v>
+        <v>-8.5</v>
       </c>
       <c r="C129">
         <v>1.31008</v>
@@ -2204,7 +2204,7 @@
         <v>43280</v>
       </c>
       <c r="B130">
-        <v>27.39999999999965</v>
+        <v>27.4</v>
       </c>
       <c r="C130">
         <v>1.31729</v>
@@ -2218,7 +2218,7 @@
         <v>43283</v>
       </c>
       <c r="B131">
-        <v>19.90000000000158</v>
+        <v>19.9</v>
       </c>
       <c r="C131">
         <v>1.31043</v>
@@ -2232,7 +2232,7 @@
         <v>43284</v>
       </c>
       <c r="B132">
-        <v>-0.7999999999985796</v>
+        <v>-0.8</v>
       </c>
       <c r="C132">
         <v>1.3173</v>
@@ -2246,7 +2246,7 @@
         <v>43285</v>
       </c>
       <c r="B133">
-        <v>-10.89999999999813</v>
+        <v>-10.9</v>
       </c>
       <c r="C133">
         <v>1.32204</v>
@@ -2260,7 +2260,7 @@
         <v>43286</v>
       </c>
       <c r="B134">
-        <v>-4.300000000001525</v>
+        <v>-4.3</v>
       </c>
       <c r="C134">
         <v>1.32247</v>
@@ -2274,7 +2274,7 @@
         <v>43287</v>
       </c>
       <c r="B135">
-        <v>-0.4000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="C135">
         <v>1.32713</v>
@@ -2288,7 +2288,7 @@
         <v>43290</v>
       </c>
       <c r="B136">
-        <v>14.30000000000264</v>
+        <v>14.3</v>
       </c>
       <c r="C136">
         <v>1.32448</v>
@@ -2302,7 +2302,7 @@
         <v>43291</v>
       </c>
       <c r="B137">
-        <v>-7.00000000000145</v>
+        <v>-7</v>
       </c>
       <c r="C137">
         <v>1.32738</v>
@@ -2316,7 +2316,7 @@
         <v>43292</v>
       </c>
       <c r="B138">
-        <v>-22.10000000000045</v>
+        <v>-22.1</v>
       </c>
       <c r="C138">
         <v>1.32692</v>
@@ -2330,7 +2330,7 @@
         <v>43293</v>
       </c>
       <c r="B139">
-        <v>4.100000000000215</v>
+        <v>4.1</v>
       </c>
       <c r="C139">
         <v>1.322</v>
@@ -2344,7 +2344,7 @@
         <v>43294</v>
       </c>
       <c r="B140">
-        <v>18.20000000000155</v>
+        <v>18.2</v>
       </c>
       <c r="C140">
         <v>1.31828</v>
@@ -2358,7 +2358,7 @@
         <v>43297</v>
       </c>
       <c r="B141">
-        <v>-38.59999999999975</v>
+        <v>-38.6</v>
       </c>
       <c r="C141">
         <v>1.32661</v>
@@ -2372,7 +2372,7 @@
         <v>43298</v>
       </c>
       <c r="B142">
-        <v>0.7000000000023654</v>
+        <v>0.7</v>
       </c>
       <c r="C142">
         <v>1.31574</v>
@@ -2386,7 +2386,7 @@
         <v>43299</v>
       </c>
       <c r="B143">
-        <v>4.499999999998394</v>
+        <v>4.5</v>
       </c>
       <c r="C143">
         <v>1.30411</v>
@@ -2400,7 +2400,7 @@
         <v>43300</v>
       </c>
       <c r="B144">
-        <v>3.40000000000007</v>
+        <v>3.4</v>
       </c>
       <c r="C144">
         <v>1.29959</v>
@@ -2414,7 +2414,7 @@
         <v>43301</v>
       </c>
       <c r="B145">
-        <v>-7.200000000000539</v>
+        <v>-7.2</v>
       </c>
       <c r="C145">
         <v>1.31062</v>
@@ -2428,7 +2428,7 @@
         <v>43304</v>
       </c>
       <c r="B146">
-        <v>4.799999999998139</v>
+        <v>4.8</v>
       </c>
       <c r="C146">
         <v>1.31085</v>
@@ -2442,7 +2442,7 @@
         <v>43305</v>
       </c>
       <c r="B147">
-        <v>10.7999999999997</v>
+        <v>10.8</v>
       </c>
       <c r="C147">
         <v>1.31421</v>
@@ -2456,7 +2456,7 @@
         <v>43306</v>
       </c>
       <c r="B148">
-        <v>6.699999999999484</v>
+        <v>6.7</v>
       </c>
       <c r="C148">
         <v>1.31433</v>
@@ -2470,7 +2470,7 @@
         <v>43307</v>
       </c>
       <c r="B149">
-        <v>22.80000000000282</v>
+        <v>22.8</v>
       </c>
       <c r="C149">
         <v>1.31279</v>
@@ -2484,7 +2484,7 @@
         <v>43308</v>
       </c>
       <c r="B150">
-        <v>5.999999999999339</v>
+        <v>6</v>
       </c>
       <c r="C150">
         <v>1.31185</v>
@@ -2498,7 +2498,7 @@
         <v>43311</v>
       </c>
       <c r="B151">
-        <v>-3.599999999996939</v>
+        <v>-3.6</v>
       </c>
       <c r="C151">
         <v>1.31488</v>
@@ -2512,7 +2512,7 @@
         <v>43312</v>
       </c>
       <c r="B152">
-        <v>-13.69999999999871</v>
+        <v>-13.7</v>
       </c>
       <c r="C152">
         <v>1.31303</v>
@@ -2526,7 +2526,7 @@
         <v>43313</v>
       </c>
       <c r="B153">
-        <v>-2.99999999999967</v>
+        <v>-3</v>
       </c>
       <c r="C153">
         <v>1.31248</v>
@@ -2540,7 +2540,7 @@
         <v>43314</v>
       </c>
       <c r="B154">
-        <v>-8.500000000000174</v>
+        <v>-8.5</v>
       </c>
       <c r="C154">
         <v>1.30394</v>
@@ -2554,7 +2554,7 @@
         <v>43315</v>
       </c>
       <c r="B155">
-        <v>11.6000000000005</v>
+        <v>11.6</v>
       </c>
       <c r="C155">
         <v>1.3004</v>
@@ -2568,7 +2568,7 @@
         <v>43318</v>
       </c>
       <c r="B156">
-        <v>-9.100000000001884</v>
+        <v>-9.1</v>
       </c>
       <c r="C156">
         <v>1.29496</v>
@@ -2582,7 +2582,7 @@
         <v>43319</v>
       </c>
       <c r="B157">
-        <v>10.20000000000021</v>
+        <v>10.2</v>
       </c>
       <c r="C157">
         <v>1.29437</v>
@@ -2596,7 +2596,7 @@
         <v>43320</v>
       </c>
       <c r="B158">
-        <v>12.99999999999857</v>
+        <v>13</v>
       </c>
       <c r="C158">
         <v>1.28717</v>
@@ -2610,7 +2610,7 @@
         <v>43321</v>
       </c>
       <c r="B159">
-        <v>-11.10000000000166</v>
+        <v>-11.1</v>
       </c>
       <c r="C159">
         <v>1.28814</v>
@@ -2624,7 +2624,7 @@
         <v>43322</v>
       </c>
       <c r="B160">
-        <v>7.200000000000539</v>
+        <v>7.2</v>
       </c>
       <c r="C160">
         <v>1.27628</v>
@@ -2638,7 +2638,7 @@
         <v>43325</v>
       </c>
       <c r="B161">
-        <v>-12.69999999999882</v>
+        <v>-12.7</v>
       </c>
       <c r="C161">
         <v>1.27883</v>
@@ -2652,7 +2652,7 @@
         <v>43326</v>
       </c>
       <c r="B162">
-        <v>-18.89999999999947</v>
+        <v>-18.9</v>
       </c>
       <c r="C162">
         <v>1.27694</v>
@@ -2666,7 +2666,7 @@
         <v>43327</v>
       </c>
       <c r="B163">
-        <v>-11.99999999999868</v>
+        <v>-12</v>
       </c>
       <c r="C163">
         <v>1.26847</v>
@@ -2680,7 +2680,7 @@
         <v>43328</v>
       </c>
       <c r="B164">
-        <v>-1.100000000000545</v>
+        <v>-1.1</v>
       </c>
       <c r="C164">
         <v>1.27291</v>
@@ -2694,7 +2694,7 @@
         <v>43329</v>
       </c>
       <c r="B165">
-        <v>7.500000000000284</v>
+        <v>7.5</v>
       </c>
       <c r="C165">
         <v>1.27286</v>
@@ -2708,7 +2708,7 @@
         <v>43332</v>
       </c>
       <c r="B166">
-        <v>-12.39999999999908</v>
+        <v>-12.4</v>
       </c>
       <c r="C166">
         <v>1.27718</v>
@@ -2722,7 +2722,7 @@
         <v>43333</v>
       </c>
       <c r="B167">
-        <v>-3.20000000000098</v>
+        <v>-3.2</v>
       </c>
       <c r="C167">
         <v>1.28678</v>
@@ -2736,7 +2736,7 @@
         <v>43334</v>
       </c>
       <c r="B168">
-        <v>-4.299999999999304</v>
+        <v>-4.3</v>
       </c>
       <c r="C168">
         <v>1.29129</v>
@@ -2750,7 +2750,7 @@
         <v>43335</v>
       </c>
       <c r="B169">
-        <v>-4.599999999999049</v>
+        <v>-4.6</v>
       </c>
       <c r="C169">
         <v>1.28388</v>
@@ -2764,7 +2764,7 @@
         <v>43336</v>
       </c>
       <c r="B170">
-        <v>1.699999999997814</v>
+        <v>1.7</v>
       </c>
       <c r="C170">
         <v>1.28557</v>
@@ -2778,7 +2778,7 @@
         <v>43339</v>
       </c>
       <c r="B171">
-        <v>0.8999999999992347</v>
+        <v>0.9</v>
       </c>
       <c r="C171">
         <v>1.28865</v>
@@ -2792,7 +2792,7 @@
         <v>43340</v>
       </c>
       <c r="B172">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C172">
         <v>1.28838</v>
@@ -2806,7 +2806,7 @@
         <v>43341</v>
       </c>
       <c r="B173">
-        <v>-10.49999999999995</v>
+        <v>-10.5</v>
       </c>
       <c r="C173">
         <v>1.29923</v>
@@ -2820,7 +2820,7 @@
         <v>43342</v>
       </c>
       <c r="B174">
-        <v>-8.300000000001084</v>
+        <v>-8.300000000000001</v>
       </c>
       <c r="C174">
         <v>1.30132</v>
@@ -2834,7 +2834,7 @@
         <v>43343</v>
       </c>
       <c r="B175">
-        <v>11.00000000000101</v>
+        <v>11</v>
       </c>
       <c r="C175">
         <v>1.29836</v>
@@ -2848,7 +2848,7 @@
         <v>43346</v>
       </c>
       <c r="B176">
-        <v>8.800000000002139</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C176">
         <v>1.28733</v>
@@ -2862,7 +2862,7 @@
         <v>43347</v>
       </c>
       <c r="B177">
-        <v>7.199999999998319</v>
+        <v>7.2</v>
       </c>
       <c r="C177">
         <v>1.28207</v>
@@ -2876,7 +2876,7 @@
         <v>43348</v>
       </c>
       <c r="B178">
-        <v>-13.00000000000079</v>
+        <v>-13</v>
       </c>
       <c r="C178">
         <v>1.29672</v>
@@ -2890,7 +2890,7 @@
         <v>43349</v>
       </c>
       <c r="B179">
-        <v>4.499999999998394</v>
+        <v>4.5</v>
       </c>
       <c r="C179">
         <v>1.29412</v>
@@ -2904,7 +2904,7 @@
         <v>43350</v>
       </c>
       <c r="B180">
-        <v>-15.99999999999824</v>
+        <v>-16</v>
       </c>
       <c r="C180">
         <v>1.29648</v>
@@ -2918,7 +2918,7 @@
         <v>43353</v>
       </c>
       <c r="B181">
-        <v>-4.499999999998394</v>
+        <v>-4.5</v>
       </c>
       <c r="C181">
         <v>1.30257</v>
@@ -2932,7 +2932,7 @@
         <v>43354</v>
       </c>
       <c r="B182">
-        <v>0.2000000000013102</v>
+        <v>0.2</v>
       </c>
       <c r="C182">
         <v>1.30008</v>
@@ -2946,7 +2946,7 @@
         <v>43355</v>
       </c>
       <c r="B183">
-        <v>-0.4000000000026205</v>
+        <v>-0.4</v>
       </c>
       <c r="C183">
         <v>1.30212</v>
@@ -2960,7 +2960,7 @@
         <v>43356</v>
       </c>
       <c r="B184">
-        <v>-6.800000000000139</v>
+        <v>-6.8</v>
       </c>
       <c r="C184">
         <v>1.3102</v>
@@ -2974,7 +2974,7 @@
         <v>43357</v>
       </c>
       <c r="B185">
-        <v>-4.699999999999704</v>
+        <v>-4.7</v>
       </c>
       <c r="C185">
         <v>1.30782</v>
@@ -2988,7 +2988,7 @@
         <v>43360</v>
       </c>
       <c r="B186">
-        <v>3.999999999999559</v>
+        <v>4</v>
       </c>
       <c r="C186">
         <v>1.31484</v>
@@ -3002,7 +3002,7 @@
         <v>43361</v>
       </c>
       <c r="B187">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C187">
         <v>1.31535</v>
@@ -3016,7 +3016,7 @@
         <v>43362</v>
       </c>
       <c r="B188">
-        <v>11.70000000000115</v>
+        <v>11.7</v>
       </c>
       <c r="C188">
         <v>1.31418</v>
@@ -3030,7 +3030,7 @@
         <v>43363</v>
       </c>
       <c r="B189">
-        <v>-7.099999999999884</v>
+        <v>-7.1</v>
       </c>
       <c r="C189">
         <v>1.32617</v>
@@ -3044,7 +3044,7 @@
         <v>43364</v>
       </c>
       <c r="B190">
-        <v>16.20000000000177</v>
+        <v>16.2</v>
       </c>
       <c r="C190">
         <v>1.30835</v>
@@ -3058,7 +3058,7 @@
         <v>43367</v>
       </c>
       <c r="B191">
-        <v>4.100000000000215</v>
+        <v>4.1</v>
       </c>
       <c r="C191">
         <v>1.31343</v>
@@ -3072,7 +3072,7 @@
         <v>43368</v>
       </c>
       <c r="B192">
-        <v>4.100000000000215</v>
+        <v>4.1</v>
       </c>
       <c r="C192">
         <v>1.31581</v>
@@ -3086,7 +3086,7 @@
         <v>43369</v>
       </c>
       <c r="B193">
-        <v>6.699999999999484</v>
+        <v>6.7</v>
       </c>
       <c r="C193">
         <v>1.31728</v>
@@ -3100,7 +3100,7 @@
         <v>43370</v>
       </c>
       <c r="B194">
-        <v>-17.89999999999958</v>
+        <v>-17.9</v>
       </c>
       <c r="C194">
         <v>1.31346</v>
@@ -3114,7 +3114,7 @@
         <v>43371</v>
       </c>
       <c r="B195">
-        <v>37.69999999999829</v>
+        <v>37.7</v>
       </c>
       <c r="C195">
         <v>1.30072</v>
@@ -3128,7 +3128,7 @@
         <v>43374</v>
       </c>
       <c r="B196">
-        <v>-19.59999999999962</v>
+        <v>-19.6</v>
       </c>
       <c r="C196">
         <v>1.3065</v>
@@ -3142,7 +3142,7 @@
         <v>43375</v>
       </c>
       <c r="B197">
-        <v>1.99999999999978</v>
+        <v>2</v>
       </c>
       <c r="C197">
         <v>1.29793</v>
@@ -3156,7 +3156,7 @@
         <v>43376</v>
       </c>
       <c r="B198">
-        <v>-11.39999999999919</v>
+        <v>-11.4</v>
       </c>
       <c r="C198">
         <v>1.30176</v>
@@ -3170,7 +3170,7 @@
         <v>43377</v>
       </c>
       <c r="B199">
-        <v>-4.900000000001015</v>
+        <v>-4.9</v>
       </c>
       <c r="C199">
         <v>1.30328</v>
@@ -3184,7 +3184,7 @@
         <v>43378</v>
       </c>
       <c r="B200">
-        <v>6.699999999999484</v>
+        <v>6.7</v>
       </c>
       <c r="C200">
         <v>1.3077</v>
@@ -3198,7 +3198,7 @@
         <v>43381</v>
       </c>
       <c r="B201">
-        <v>-4.999999999999449</v>
+        <v>-5</v>
       </c>
       <c r="C201">
         <v>1.30684</v>
@@ -3212,7 +3212,7 @@
         <v>43382</v>
       </c>
       <c r="B202">
-        <v>-6.399999999999739</v>
+        <v>-6.4</v>
       </c>
       <c r="C202">
         <v>1.30916</v>
@@ -3226,7 +3226,7 @@
         <v>43383</v>
       </c>
       <c r="B203">
-        <v>9.099999999999664</v>
+        <v>9.1</v>
       </c>
       <c r="C203">
         <v>1.31918</v>
@@ -3240,7 +3240,7 @@
         <v>43384</v>
       </c>
       <c r="B204">
-        <v>-15.10000000000122</v>
+        <v>-15.1</v>
       </c>
       <c r="C204">
         <v>1.32242</v>
@@ -3254,7 +3254,7 @@
         <v>43385</v>
       </c>
       <c r="B205">
-        <v>-27.60000000000096</v>
+        <v>-27.6</v>
       </c>
       <c r="C205">
         <v>1.31847</v>
@@ -3268,7 +3268,7 @@
         <v>43388</v>
       </c>
       <c r="B206">
-        <v>8.099999999997554</v>
+        <v>8.1</v>
       </c>
       <c r="C206">
         <v>1.31367</v>
@@ -3282,7 +3282,7 @@
         <v>43389</v>
       </c>
       <c r="B207">
-        <v>0.4000000000026205</v>
+        <v>0.4</v>
       </c>
       <c r="C207">
         <v>1.32113</v>
@@ -3296,7 +3296,7 @@
         <v>43390</v>
       </c>
       <c r="B208">
-        <v>-0.9999999999998899</v>
+        <v>-1</v>
       </c>
       <c r="C208">
         <v>1.31349</v>
@@ -3310,7 +3310,7 @@
         <v>43391</v>
       </c>
       <c r="B209">
-        <v>-18.50000000000129</v>
+        <v>-18.5</v>
       </c>
       <c r="C209">
         <v>1.30882</v>
@@ -3324,7 +3324,7 @@
         <v>43392</v>
       </c>
       <c r="B210">
-        <v>-2.99999999999967</v>
+        <v>-3</v>
       </c>
       <c r="C210">
         <v>1.30471</v>
@@ -3338,7 +3338,7 @@
         <v>43395</v>
       </c>
       <c r="B211">
-        <v>-1.6000000000016</v>
+        <v>-1.6</v>
       </c>
       <c r="C211">
         <v>1.2974</v>
@@ -3352,7 +3352,7 @@
         <v>43396</v>
       </c>
       <c r="B212">
-        <v>-6.200000000000649</v>
+        <v>-6.2</v>
       </c>
       <c r="C212">
         <v>1.29793</v>
@@ -3366,7 +3366,7 @@
         <v>43397</v>
       </c>
       <c r="B213">
-        <v>-11.69999999999893</v>
+        <v>-11.7</v>
       </c>
       <c r="C213">
         <v>1.29219</v>
@@ -3380,7 +3380,7 @@
         <v>43398</v>
       </c>
       <c r="B214">
-        <v>-16.19999999999955</v>
+        <v>-16.2</v>
       </c>
       <c r="C214">
         <v>1.28283</v>
@@ -3394,7 +3394,7 @@
         <v>43399</v>
       </c>
       <c r="B215">
-        <v>5.899999999998684</v>
+        <v>5.9</v>
       </c>
       <c r="C215">
         <v>1.28125</v>
@@ -3408,7 +3408,7 @@
         <v>43402</v>
       </c>
       <c r="B216">
-        <v>3.900000000001125</v>
+        <v>3.9</v>
       </c>
       <c r="C216">
         <v>1.28079</v>
@@ -3422,7 +3422,7 @@
         <v>43403</v>
       </c>
       <c r="B217">
-        <v>-19.10000000000078</v>
+        <v>-19.1</v>
       </c>
       <c r="C217">
         <v>1.27607</v>
@@ -3436,7 +3436,7 @@
         <v>43404</v>
       </c>
       <c r="B218">
-        <v>-6.699999999999484</v>
+        <v>-6.7</v>
       </c>
       <c r="C218">
         <v>1.27741</v>
@@ -3450,7 +3450,7 @@
         <v>43405</v>
       </c>
       <c r="B219">
-        <v>4.299999999999304</v>
+        <v>4.3</v>
       </c>
       <c r="C219">
         <v>1.2939</v>
@@ -3464,7 +3464,7 @@
         <v>43406</v>
       </c>
       <c r="B220">
-        <v>-14.89999999999991</v>
+        <v>-14.9</v>
       </c>
       <c r="C220">
         <v>1.29965</v>
@@ -3478,7 +3478,7 @@
         <v>43409</v>
       </c>
       <c r="B221">
-        <v>-8.099999999999774</v>
+        <v>-8.1</v>
       </c>
       <c r="C221">
         <v>1.30308</v>
@@ -3492,7 +3492,7 @@
         <v>43410</v>
       </c>
       <c r="B222">
-        <v>-0.7000000000023654</v>
+        <v>-0.7</v>
       </c>
       <c r="C222">
         <v>1.30781</v>
@@ -3506,7 +3506,7 @@
         <v>43411</v>
       </c>
       <c r="B223">
-        <v>-20.60000000000173</v>
+        <v>-20.6</v>
       </c>
       <c r="C223">
         <v>1.31537</v>
@@ -3520,7 +3520,7 @@
         <v>43412</v>
       </c>
       <c r="B224">
-        <v>5.60000000000116</v>
+        <v>5.6</v>
       </c>
       <c r="C224">
         <v>1.31164</v>
@@ -3534,7 +3534,7 @@
         <v>43413</v>
       </c>
       <c r="B225">
-        <v>-13.09999999999922</v>
+        <v>-13.1</v>
       </c>
       <c r="C225">
         <v>1.30403</v>
@@ -3548,7 +3548,7 @@
         <v>43416</v>
       </c>
       <c r="B226">
-        <v>-26.10000000000001</v>
+        <v>-26.1</v>
       </c>
       <c r="C226">
         <v>1.28896</v>
@@ -3562,7 +3562,7 @@
         <v>43417</v>
       </c>
       <c r="B227">
-        <v>42.39999999999799</v>
+        <v>42.4</v>
       </c>
       <c r="C227">
         <v>1.29509</v>
@@ -3576,7 +3576,7 @@
         <v>43418</v>
       </c>
       <c r="B228">
-        <v>24.90000000000103</v>
+        <v>24.9</v>
       </c>
       <c r="C228">
         <v>1.29775</v>
@@ -3590,7 +3590,7 @@
         <v>43419</v>
       </c>
       <c r="B229">
-        <v>-18.19999999999933</v>
+        <v>-18.2</v>
       </c>
       <c r="C229">
         <v>1.27949</v>
@@ -3604,7 +3604,7 @@
         <v>43420</v>
       </c>
       <c r="B230">
-        <v>-14.60000000000017</v>
+        <v>-14.6</v>
       </c>
       <c r="C230">
         <v>1.28535</v>
@@ -3618,7 +3618,7 @@
         <v>43423</v>
       </c>
       <c r="B231">
-        <v>5.299999999999194</v>
+        <v>5.3</v>
       </c>
       <c r="C231">
         <v>1.28593</v>
@@ -3632,7 +3632,7 @@
         <v>43424</v>
       </c>
       <c r="B232">
-        <v>-5.500000000000504</v>
+        <v>-5.5</v>
       </c>
       <c r="C232">
         <v>1.28275</v>
@@ -3646,7 +3646,7 @@
         <v>43425</v>
       </c>
       <c r="B233">
-        <v>-30.69999999999906</v>
+        <v>-30.7</v>
       </c>
       <c r="C233">
         <v>1.28069</v>
@@ -3660,7 +3660,7 @@
         <v>43426</v>
       </c>
       <c r="B234">
-        <v>8.399999999999519</v>
+        <v>8.4</v>
       </c>
       <c r="C234">
         <v>1.28615</v>
@@ -3674,7 +3674,7 @@
         <v>43427</v>
       </c>
       <c r="B235">
-        <v>-18.00000000000024</v>
+        <v>-18</v>
       </c>
       <c r="C235">
         <v>1.28248</v>
@@ -3688,7 +3688,7 @@
         <v>43430</v>
       </c>
       <c r="B236">
-        <v>-10.20000000000243</v>
+        <v>-10.2</v>
       </c>
       <c r="C236">
         <v>1.2835</v>
@@ -3702,7 +3702,7 @@
         <v>43431</v>
       </c>
       <c r="B237">
-        <v>-16.19999999999955</v>
+        <v>-16.2</v>
       </c>
       <c r="C237">
         <v>1.27535</v>
@@ -3716,7 +3716,7 @@
         <v>43432</v>
       </c>
       <c r="B238">
-        <v>-20.7999999999986</v>
+        <v>-20.8</v>
       </c>
       <c r="C238">
         <v>1.27723</v>
@@ -3730,7 +3730,7 @@
         <v>43433</v>
       </c>
       <c r="B239">
-        <v>2.100000000000435</v>
+        <v>2.1</v>
       </c>
       <c r="C239">
         <v>1.27779</v>
@@ -3744,7 +3744,7 @@
         <v>43434</v>
       </c>
       <c r="B240">
-        <v>11.6000000000005</v>
+        <v>11.6</v>
       </c>
       <c r="C240">
         <v>1.2751</v>
@@ -3758,7 +3758,7 @@
         <v>43437</v>
       </c>
       <c r="B241">
-        <v>8.600000000000829</v>
+        <v>8.6</v>
       </c>
       <c r="C241">
         <v>1.27294</v>
@@ -3772,7 +3772,7 @@
         <v>43438</v>
       </c>
       <c r="B242">
-        <v>-17.100000000001</v>
+        <v>-17.1</v>
       </c>
       <c r="C242">
         <v>1.27432</v>
@@ -3786,7 +3786,7 @@
         <v>43439</v>
       </c>
       <c r="B243">
-        <v>6.399999999999739</v>
+        <v>6.4</v>
       </c>
       <c r="C243">
         <v>1.27275</v>
@@ -3800,7 +3800,7 @@
         <v>43440</v>
       </c>
       <c r="B244">
-        <v>-18.40000000000064</v>
+        <v>-18.4</v>
       </c>
       <c r="C244">
         <v>1.2798</v>
@@ -3814,7 +3814,7 @@
         <v>43441</v>
       </c>
       <c r="B245">
-        <v>17.30000000000231</v>
+        <v>17.3</v>
       </c>
       <c r="C245">
         <v>1.27334</v>
@@ -3828,7 +3828,7 @@
         <v>43444</v>
       </c>
       <c r="B246">
-        <v>-119.6000000000019</v>
+        <v>-119.6</v>
       </c>
       <c r="C246">
         <v>1.26455</v>
@@ -3842,7 +3842,7 @@
         <v>43445</v>
       </c>
       <c r="B247">
-        <v>-46.90000000000083</v>
+        <v>-46.9</v>
       </c>
       <c r="C247">
         <v>1.2556</v>
@@ -3856,7 +3856,7 @@
         <v>43446</v>
       </c>
       <c r="B248">
-        <v>15.39999999999875</v>
+        <v>15.4</v>
       </c>
       <c r="C248">
         <v>1.2642</v>
@@ -3870,7 +3870,7 @@
         <v>43447</v>
       </c>
       <c r="B249">
-        <v>-8.500000000000174</v>
+        <v>-8.5</v>
       </c>
       <c r="C249">
         <v>1.26256</v>
@@ -3884,7 +3884,7 @@
         <v>43448</v>
       </c>
       <c r="B250">
-        <v>9.399999999999409</v>
+        <v>9.4</v>
       </c>
       <c r="C250">
         <v>1.25487</v>
@@ -3898,7 +3898,7 @@
         <v>43451</v>
       </c>
       <c r="B251">
-        <v>-1.59999999999938</v>
+        <v>-1.6</v>
       </c>
       <c r="C251">
         <v>1.26081</v>
@@ -3912,7 +3912,7 @@
         <v>43452</v>
       </c>
       <c r="B252">
-        <v>-22.60000000000151</v>
+        <v>-22.6</v>
       </c>
       <c r="C252">
         <v>1.26569</v>
@@ -3926,7 +3926,7 @@
         <v>43453</v>
       </c>
       <c r="B253">
-        <v>-21.80000000000071</v>
+        <v>-21.8</v>
       </c>
       <c r="C253">
         <v>1.26686</v>
@@ -3940,7 +3940,7 @@
         <v>43454</v>
       </c>
       <c r="B254">
-        <v>-5.699999999999594</v>
+        <v>-5.7</v>
       </c>
       <c r="C254">
         <v>1.26416</v>
@@ -3954,7 +3954,7 @@
         <v>43455</v>
       </c>
       <c r="B255">
-        <v>20.3999999999982</v>
+        <v>20.4</v>
       </c>
       <c r="C255">
         <v>1.26465</v>
@@ -3968,7 +3968,7 @@
         <v>43458</v>
       </c>
       <c r="B256">
-        <v>5.100000000000104</v>
+        <v>5.1</v>
       </c>
       <c r="C256">
         <v>1.27124</v>
@@ -3982,7 +3982,7 @@
         <v>43460</v>
       </c>
       <c r="B257">
-        <v>-17.40000000000297</v>
+        <v>-17.4</v>
       </c>
       <c r="C257">
         <v>1.26907</v>
@@ -3996,7 +3996,7 @@
         <v>43461</v>
       </c>
       <c r="B258">
-        <v>-26.00000000000158</v>
+        <v>-26</v>
       </c>
       <c r="C258">
         <v>1.26583</v>
@@ -4010,7 +4010,7 @@
         <v>43462</v>
       </c>
       <c r="B259">
-        <v>1.300000000001855</v>
+        <v>1.3</v>
       </c>
       <c r="C259">
         <v>1.26818</v>
@@ -4024,7 +4024,7 @@
         <v>43465</v>
       </c>
       <c r="B260">
-        <v>-73.39999999999903</v>
+        <v>-73.40000000000001</v>
       </c>
       <c r="C260">
         <v>1.28061</v>
@@ -4040,7 +4040,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4062,7 +4062,7 @@
         <v>43104</v>
       </c>
       <c r="B2">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C2">
         <v>1.35534</v>
@@ -4076,7 +4076,7 @@
         <v>43123</v>
       </c>
       <c r="B3">
-        <v>-0.5999999999972694</v>
+        <v>-0.6</v>
       </c>
       <c r="C3">
         <v>1.40138</v>
@@ -4090,7 +4090,7 @@
         <v>43133</v>
       </c>
       <c r="B4">
-        <v>-2.900000000001235</v>
+        <v>-2.9</v>
       </c>
       <c r="C4">
         <v>1.41291</v>
@@ -4104,7 +4104,7 @@
         <v>43136</v>
       </c>
       <c r="B5">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C5">
         <v>1.40236</v>
@@ -4118,7 +4118,7 @@
         <v>43143</v>
       </c>
       <c r="B6">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C6">
         <v>1.38067</v>
@@ -4132,7 +4132,7 @@
         <v>43153</v>
       </c>
       <c r="B7">
-        <v>-1.699999999997814</v>
+        <v>-1.7</v>
       </c>
       <c r="C7">
         <v>1.39413</v>
@@ -4146,7 +4146,7 @@
         <v>43165</v>
       </c>
       <c r="B8">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C8">
         <v>1.38924</v>
@@ -4160,7 +4160,7 @@
         <v>43180</v>
       </c>
       <c r="B9">
-        <v>-1.399999999998069</v>
+        <v>-1.4</v>
       </c>
       <c r="C9">
         <v>1.40705</v>
@@ -4174,7 +4174,7 @@
         <v>43189</v>
       </c>
       <c r="B10">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C10">
         <v>1.40365</v>
@@ -4188,7 +4188,7 @@
         <v>43192</v>
       </c>
       <c r="B11">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C11">
         <v>1.40542</v>
@@ -4202,7 +4202,7 @@
         <v>43201</v>
       </c>
       <c r="B12">
-        <v>-1.500000000000945</v>
+        <v>-1.5</v>
       </c>
       <c r="C12">
         <v>1.42048</v>
@@ -4216,7 +4216,7 @@
         <v>43207</v>
       </c>
       <c r="B13">
-        <v>-1.899999999999125</v>
+        <v>-1.9</v>
       </c>
       <c r="C13">
         <v>1.43095</v>
@@ -4230,7 +4230,7 @@
         <v>43220</v>
       </c>
       <c r="B14">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C14">
         <v>1.37687</v>
@@ -4244,7 +4244,7 @@
         <v>43257</v>
       </c>
       <c r="B15">
-        <v>-2.19999999999887</v>
+        <v>-2.2</v>
       </c>
       <c r="C15">
         <v>1.34273</v>
@@ -4258,7 +4258,7 @@
         <v>43284</v>
       </c>
       <c r="B16">
-        <v>-0.7999999999985796</v>
+        <v>-0.8</v>
       </c>
       <c r="C16">
         <v>1.3173</v>
@@ -4272,7 +4272,7 @@
         <v>43287</v>
       </c>
       <c r="B17">
-        <v>-0.4000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="C17">
         <v>1.32713</v>
@@ -4283,141 +4283,113 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>43313</v>
+        <v>43328</v>
       </c>
       <c r="B18">
-        <v>-2.99999999999967</v>
+        <v>-1.1</v>
       </c>
       <c r="C18">
-        <v>1.31248</v>
+        <v>1.27291</v>
       </c>
       <c r="D18">
-        <v>1.31218</v>
+        <v>1.2728</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>43328</v>
+        <v>43340</v>
       </c>
       <c r="B19">
-        <v>-1.100000000000545</v>
+        <v>-2</v>
       </c>
       <c r="C19">
-        <v>1.27291</v>
+        <v>1.28838</v>
       </c>
       <c r="D19">
-        <v>1.2728</v>
+        <v>1.28818</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>43340</v>
+        <v>43355</v>
       </c>
       <c r="B20">
-        <v>-1.99999999999978</v>
+        <v>-0.4</v>
       </c>
       <c r="C20">
-        <v>1.28838</v>
+        <v>1.30212</v>
       </c>
       <c r="D20">
-        <v>1.28818</v>
+        <v>1.30208</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>43355</v>
+        <v>43361</v>
       </c>
       <c r="B21">
-        <v>-0.4000000000026205</v>
+        <v>-2.6</v>
       </c>
       <c r="C21">
-        <v>1.30212</v>
+        <v>1.31535</v>
       </c>
       <c r="D21">
-        <v>1.30208</v>
+        <v>1.31509</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>43361</v>
+        <v>43390</v>
       </c>
       <c r="B22">
-        <v>-2.60000000000149</v>
+        <v>-1</v>
       </c>
       <c r="C22">
-        <v>1.31535</v>
+        <v>1.31349</v>
       </c>
       <c r="D22">
-        <v>1.31509</v>
+        <v>1.31339</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>43390</v>
+        <v>43395</v>
       </c>
       <c r="B23">
-        <v>-0.9999999999998899</v>
+        <v>-1.6</v>
       </c>
       <c r="C23">
-        <v>1.31349</v>
+        <v>1.2974</v>
       </c>
       <c r="D23">
-        <v>1.31339</v>
+        <v>1.29724</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>43392</v>
+        <v>43410</v>
       </c>
       <c r="B24">
-        <v>-2.99999999999967</v>
+        <v>-0.7</v>
       </c>
       <c r="C24">
-        <v>1.30471</v>
+        <v>1.30781</v>
       </c>
       <c r="D24">
-        <v>1.30441</v>
+        <v>1.30774</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>43395</v>
+        <v>43451</v>
       </c>
       <c r="B25">
-        <v>-1.6000000000016</v>
+        <v>-1.6</v>
       </c>
       <c r="C25">
-        <v>1.2974</v>
+        <v>1.26081</v>
       </c>
       <c r="D25">
-        <v>1.29724</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2">
-        <v>43410</v>
-      </c>
-      <c r="B26">
-        <v>-0.7000000000023654</v>
-      </c>
-      <c r="C26">
-        <v>1.30781</v>
-      </c>
-      <c r="D26">
-        <v>1.30774</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2">
-        <v>43451</v>
-      </c>
-      <c r="B27">
-        <v>-1.59999999999938</v>
-      </c>
-      <c r="C27">
-        <v>1.26081</v>
-      </c>
-      <c r="D27">
         <v>1.26065</v>
       </c>
     </row>
@@ -4428,7 +4400,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4450,7 +4422,7 @@
         <v>43104</v>
       </c>
       <c r="B2">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C2">
         <v>1.35534</v>
@@ -4464,7 +4436,7 @@
         <v>43110</v>
       </c>
       <c r="B3">
-        <v>-3.60000000000138</v>
+        <v>-3.6</v>
       </c>
       <c r="C3">
         <v>1.35315</v>
@@ -4478,7 +4450,7 @@
         <v>43123</v>
       </c>
       <c r="B4">
-        <v>-0.5999999999972694</v>
+        <v>-0.6</v>
       </c>
       <c r="C4">
         <v>1.40138</v>
@@ -4492,7 +4464,7 @@
         <v>43133</v>
       </c>
       <c r="B5">
-        <v>-2.900000000001235</v>
+        <v>-2.9</v>
       </c>
       <c r="C5">
         <v>1.41291</v>
@@ -4506,7 +4478,7 @@
         <v>43136</v>
       </c>
       <c r="B6">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C6">
         <v>1.40236</v>
@@ -4520,7 +4492,7 @@
         <v>43143</v>
       </c>
       <c r="B7">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C7">
         <v>1.38067</v>
@@ -4534,7 +4506,7 @@
         <v>43147</v>
       </c>
       <c r="B8">
-        <v>-3.199999999998759</v>
+        <v>-3.2</v>
       </c>
       <c r="C8">
         <v>1.40462</v>
@@ -4548,7 +4520,7 @@
         <v>43153</v>
       </c>
       <c r="B9">
-        <v>-1.699999999997814</v>
+        <v>-1.7</v>
       </c>
       <c r="C9">
         <v>1.39413</v>
@@ -4562,7 +4534,7 @@
         <v>43161</v>
       </c>
       <c r="B10">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C10">
         <v>1.37769</v>
@@ -4576,7 +4548,7 @@
         <v>43165</v>
       </c>
       <c r="B11">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C11">
         <v>1.38924</v>
@@ -4590,7 +4562,7 @@
         <v>43180</v>
       </c>
       <c r="B12">
-        <v>-1.399999999998069</v>
+        <v>-1.4</v>
       </c>
       <c r="C12">
         <v>1.40705</v>
@@ -4604,7 +4576,7 @@
         <v>43189</v>
       </c>
       <c r="B13">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C13">
         <v>1.40365</v>
@@ -4618,7 +4590,7 @@
         <v>43192</v>
       </c>
       <c r="B14">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C14">
         <v>1.40542</v>
@@ -4629,295 +4601,281 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>43194</v>
+        <v>43201</v>
       </c>
       <c r="B15">
-        <v>-3.999999999999559</v>
+        <v>-1.5</v>
       </c>
       <c r="C15">
-        <v>1.40841</v>
+        <v>1.42048</v>
       </c>
       <c r="D15">
-        <v>1.40801</v>
+        <v>1.42033</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>43201</v>
+        <v>43207</v>
       </c>
       <c r="B16">
-        <v>-1.500000000000945</v>
+        <v>-1.9</v>
       </c>
       <c r="C16">
-        <v>1.42048</v>
+        <v>1.43095</v>
       </c>
       <c r="D16">
-        <v>1.42033</v>
+        <v>1.43076</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>43207</v>
+        <v>43220</v>
       </c>
       <c r="B17">
-        <v>-1.899999999999125</v>
+        <v>-2</v>
       </c>
       <c r="C17">
-        <v>1.43095</v>
+        <v>1.37687</v>
       </c>
       <c r="D17">
-        <v>1.43076</v>
+        <v>1.37667</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>43220</v>
+        <v>43230</v>
       </c>
       <c r="B18">
-        <v>-1.99999999999978</v>
+        <v>-3.9</v>
       </c>
       <c r="C18">
-        <v>1.37687</v>
+        <v>1.34723</v>
       </c>
       <c r="D18">
-        <v>1.37667</v>
+        <v>1.34684</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>43230</v>
+        <v>43257</v>
       </c>
       <c r="B19">
-        <v>-3.899999999998904</v>
+        <v>-2.2</v>
       </c>
       <c r="C19">
-        <v>1.34723</v>
+        <v>1.34273</v>
       </c>
       <c r="D19">
-        <v>1.34684</v>
+        <v>1.34251</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>43257</v>
+        <v>43262</v>
       </c>
       <c r="B20">
-        <v>-2.19999999999887</v>
+        <v>-3.6</v>
       </c>
       <c r="C20">
-        <v>1.34273</v>
+        <v>1.33961</v>
       </c>
       <c r="D20">
-        <v>1.34251</v>
+        <v>1.33925</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>43262</v>
+        <v>43284</v>
       </c>
       <c r="B21">
-        <v>-3.599999999999159</v>
+        <v>-0.8</v>
       </c>
       <c r="C21">
-        <v>1.33961</v>
+        <v>1.3173</v>
       </c>
       <c r="D21">
-        <v>1.33925</v>
+        <v>1.31722</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>43284</v>
+        <v>43287</v>
       </c>
       <c r="B22">
-        <v>-0.7999999999985796</v>
+        <v>-0.4</v>
       </c>
       <c r="C22">
-        <v>1.3173</v>
+        <v>1.32713</v>
       </c>
       <c r="D22">
-        <v>1.31722</v>
+        <v>1.32709</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>43287</v>
+        <v>43311</v>
       </c>
       <c r="B23">
-        <v>-0.4000000000004</v>
+        <v>-3.6</v>
       </c>
       <c r="C23">
-        <v>1.32713</v>
+        <v>1.31488</v>
       </c>
       <c r="D23">
-        <v>1.32709</v>
+        <v>1.31452</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>43311</v>
+        <v>43313</v>
       </c>
       <c r="B24">
-        <v>-3.599999999996939</v>
+        <v>-3</v>
       </c>
       <c r="C24">
-        <v>1.31488</v>
+        <v>1.31248</v>
       </c>
       <c r="D24">
-        <v>1.31452</v>
+        <v>1.31218</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>43313</v>
+        <v>43328</v>
       </c>
       <c r="B25">
-        <v>-2.99999999999967</v>
+        <v>-1.1</v>
       </c>
       <c r="C25">
-        <v>1.31248</v>
+        <v>1.27291</v>
       </c>
       <c r="D25">
-        <v>1.31218</v>
+        <v>1.2728</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>43328</v>
+        <v>43333</v>
       </c>
       <c r="B26">
-        <v>-1.100000000000545</v>
+        <v>-3.2</v>
       </c>
       <c r="C26">
-        <v>1.27291</v>
+        <v>1.28678</v>
       </c>
       <c r="D26">
-        <v>1.2728</v>
+        <v>1.28646</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>43333</v>
+        <v>43340</v>
       </c>
       <c r="B27">
-        <v>-3.20000000000098</v>
+        <v>-2</v>
       </c>
       <c r="C27">
-        <v>1.28678</v>
+        <v>1.28838</v>
       </c>
       <c r="D27">
-        <v>1.28646</v>
+        <v>1.28818</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>43340</v>
+        <v>43355</v>
       </c>
       <c r="B28">
-        <v>-1.99999999999978</v>
+        <v>-0.4</v>
       </c>
       <c r="C28">
-        <v>1.28838</v>
+        <v>1.30212</v>
       </c>
       <c r="D28">
-        <v>1.28818</v>
+        <v>1.30208</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>43355</v>
+        <v>43361</v>
       </c>
       <c r="B29">
-        <v>-0.4000000000026205</v>
+        <v>-2.6</v>
       </c>
       <c r="C29">
-        <v>1.30212</v>
+        <v>1.31535</v>
       </c>
       <c r="D29">
-        <v>1.30208</v>
+        <v>1.31509</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>43361</v>
+        <v>43390</v>
       </c>
       <c r="B30">
-        <v>-2.60000000000149</v>
+        <v>-1</v>
       </c>
       <c r="C30">
-        <v>1.31535</v>
+        <v>1.31349</v>
       </c>
       <c r="D30">
-        <v>1.31509</v>
+        <v>1.31339</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>43390</v>
+        <v>43392</v>
       </c>
       <c r="B31">
-        <v>-0.9999999999998899</v>
+        <v>-3</v>
       </c>
       <c r="C31">
-        <v>1.31349</v>
+        <v>1.30471</v>
       </c>
       <c r="D31">
-        <v>1.31339</v>
+        <v>1.30441</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>43392</v>
+        <v>43395</v>
       </c>
       <c r="B32">
-        <v>-2.99999999999967</v>
+        <v>-1.6</v>
       </c>
       <c r="C32">
-        <v>1.30471</v>
+        <v>1.2974</v>
       </c>
       <c r="D32">
-        <v>1.30441</v>
+        <v>1.29724</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>43395</v>
+        <v>43410</v>
       </c>
       <c r="B33">
-        <v>-1.6000000000016</v>
+        <v>-0.7</v>
       </c>
       <c r="C33">
-        <v>1.2974</v>
+        <v>1.30781</v>
       </c>
       <c r="D33">
-        <v>1.29724</v>
+        <v>1.30774</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>43410</v>
+        <v>43451</v>
       </c>
       <c r="B34">
-        <v>-0.7000000000023654</v>
+        <v>-1.6</v>
       </c>
       <c r="C34">
-        <v>1.30781</v>
+        <v>1.26081</v>
       </c>
       <c r="D34">
-        <v>1.30774</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2">
-        <v>43451</v>
-      </c>
-      <c r="B35">
-        <v>-1.59999999999938</v>
-      </c>
-      <c r="C35">
-        <v>1.26081</v>
-      </c>
-      <c r="D35">
         <v>1.26065</v>
       </c>
     </row>
@@ -4928,7 +4886,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4950,7 +4908,7 @@
         <v>43104</v>
       </c>
       <c r="B2">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C2">
         <v>1.35534</v>
@@ -4964,7 +4922,7 @@
         <v>43110</v>
       </c>
       <c r="B3">
-        <v>-3.60000000000138</v>
+        <v>-3.6</v>
       </c>
       <c r="C3">
         <v>1.35315</v>
@@ -4978,7 +4936,7 @@
         <v>43123</v>
       </c>
       <c r="B4">
-        <v>-0.5999999999972694</v>
+        <v>-0.6</v>
       </c>
       <c r="C4">
         <v>1.40138</v>
@@ -4992,7 +4950,7 @@
         <v>43133</v>
       </c>
       <c r="B5">
-        <v>-2.900000000001235</v>
+        <v>-2.9</v>
       </c>
       <c r="C5">
         <v>1.41291</v>
@@ -5006,7 +4964,7 @@
         <v>43136</v>
       </c>
       <c r="B6">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C6">
         <v>1.40236</v>
@@ -5020,7 +4978,7 @@
         <v>43143</v>
       </c>
       <c r="B7">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C7">
         <v>1.38067</v>
@@ -5034,7 +4992,7 @@
         <v>43147</v>
       </c>
       <c r="B8">
-        <v>-3.199999999998759</v>
+        <v>-3.2</v>
       </c>
       <c r="C8">
         <v>1.40462</v>
@@ -5048,7 +5006,7 @@
         <v>43153</v>
       </c>
       <c r="B9">
-        <v>-1.699999999997814</v>
+        <v>-1.7</v>
       </c>
       <c r="C9">
         <v>1.39413</v>
@@ -5062,7 +5020,7 @@
         <v>43161</v>
       </c>
       <c r="B10">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C10">
         <v>1.37769</v>
@@ -5076,7 +5034,7 @@
         <v>43165</v>
       </c>
       <c r="B11">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C11">
         <v>1.38924</v>
@@ -5090,7 +5048,7 @@
         <v>43180</v>
       </c>
       <c r="B12">
-        <v>-1.399999999998069</v>
+        <v>-1.4</v>
       </c>
       <c r="C12">
         <v>1.40705</v>
@@ -5104,7 +5062,7 @@
         <v>43189</v>
       </c>
       <c r="B13">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C13">
         <v>1.40365</v>
@@ -5118,7 +5076,7 @@
         <v>43192</v>
       </c>
       <c r="B14">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C14">
         <v>1.40542</v>
@@ -5132,7 +5090,7 @@
         <v>43194</v>
       </c>
       <c r="B15">
-        <v>-3.999999999999559</v>
+        <v>-4</v>
       </c>
       <c r="C15">
         <v>1.40841</v>
@@ -5146,7 +5104,7 @@
         <v>43201</v>
       </c>
       <c r="B16">
-        <v>-1.500000000000945</v>
+        <v>-1.5</v>
       </c>
       <c r="C16">
         <v>1.42048</v>
@@ -5160,7 +5118,7 @@
         <v>43207</v>
       </c>
       <c r="B17">
-        <v>-1.899999999999125</v>
+        <v>-1.9</v>
       </c>
       <c r="C17">
         <v>1.43095</v>
@@ -5174,7 +5132,7 @@
         <v>43214</v>
       </c>
       <c r="B18">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C18">
         <v>1.39644</v>
@@ -5188,7 +5146,7 @@
         <v>43220</v>
       </c>
       <c r="B19">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C19">
         <v>1.37687</v>
@@ -5202,7 +5160,7 @@
         <v>43230</v>
       </c>
       <c r="B20">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C20">
         <v>1.34723</v>
@@ -5216,7 +5174,7 @@
         <v>43236</v>
       </c>
       <c r="B21">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C21">
         <v>1.34873</v>
@@ -5230,7 +5188,7 @@
         <v>43257</v>
       </c>
       <c r="B22">
-        <v>-2.19999999999887</v>
+        <v>-2.2</v>
       </c>
       <c r="C22">
         <v>1.34273</v>
@@ -5244,7 +5202,7 @@
         <v>43262</v>
       </c>
       <c r="B23">
-        <v>-3.599999999999159</v>
+        <v>-3.6</v>
       </c>
       <c r="C23">
         <v>1.33961</v>
@@ -5258,7 +5216,7 @@
         <v>43284</v>
       </c>
       <c r="B24">
-        <v>-0.7999999999985796</v>
+        <v>-0.8</v>
       </c>
       <c r="C24">
         <v>1.3173</v>
@@ -5272,7 +5230,7 @@
         <v>43286</v>
       </c>
       <c r="B25">
-        <v>-4.300000000001525</v>
+        <v>-4.3</v>
       </c>
       <c r="C25">
         <v>1.32247</v>
@@ -5286,7 +5244,7 @@
         <v>43287</v>
       </c>
       <c r="B26">
-        <v>-0.4000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="C26">
         <v>1.32713</v>
@@ -5300,7 +5258,7 @@
         <v>43311</v>
       </c>
       <c r="B27">
-        <v>-3.599999999996939</v>
+        <v>-3.6</v>
       </c>
       <c r="C27">
         <v>1.31488</v>
@@ -5314,7 +5272,7 @@
         <v>43313</v>
       </c>
       <c r="B28">
-        <v>-2.99999999999967</v>
+        <v>-3</v>
       </c>
       <c r="C28">
         <v>1.31248</v>
@@ -5328,7 +5286,7 @@
         <v>43328</v>
       </c>
       <c r="B29">
-        <v>-1.100000000000545</v>
+        <v>-1.1</v>
       </c>
       <c r="C29">
         <v>1.27291</v>
@@ -5342,7 +5300,7 @@
         <v>43333</v>
       </c>
       <c r="B30">
-        <v>-3.20000000000098</v>
+        <v>-3.2</v>
       </c>
       <c r="C30">
         <v>1.28678</v>
@@ -5356,7 +5314,7 @@
         <v>43334</v>
       </c>
       <c r="B31">
-        <v>-4.299999999999304</v>
+        <v>-4.3</v>
       </c>
       <c r="C31">
         <v>1.29129</v>
@@ -5370,7 +5328,7 @@
         <v>43335</v>
       </c>
       <c r="B32">
-        <v>-4.599999999999049</v>
+        <v>-4.6</v>
       </c>
       <c r="C32">
         <v>1.28388</v>
@@ -5384,7 +5342,7 @@
         <v>43340</v>
       </c>
       <c r="B33">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C33">
         <v>1.28838</v>
@@ -5398,7 +5356,7 @@
         <v>43353</v>
       </c>
       <c r="B34">
-        <v>-4.499999999998394</v>
+        <v>-4.5</v>
       </c>
       <c r="C34">
         <v>1.30257</v>
@@ -5412,7 +5370,7 @@
         <v>43355</v>
       </c>
       <c r="B35">
-        <v>-0.4000000000026205</v>
+        <v>-0.4</v>
       </c>
       <c r="C35">
         <v>1.30212</v>
@@ -5426,7 +5384,7 @@
         <v>43357</v>
       </c>
       <c r="B36">
-        <v>-4.699999999999704</v>
+        <v>-4.7</v>
       </c>
       <c r="C36">
         <v>1.30782</v>
@@ -5440,7 +5398,7 @@
         <v>43361</v>
       </c>
       <c r="B37">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C37">
         <v>1.31535</v>
@@ -5454,7 +5412,7 @@
         <v>43377</v>
       </c>
       <c r="B38">
-        <v>-4.900000000001015</v>
+        <v>-4.9</v>
       </c>
       <c r="C38">
         <v>1.30328</v>
@@ -5465,85 +5423,71 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>43381</v>
+        <v>43390</v>
       </c>
       <c r="B39">
-        <v>-4.999999999999449</v>
+        <v>-1</v>
       </c>
       <c r="C39">
-        <v>1.30684</v>
+        <v>1.31349</v>
       </c>
       <c r="D39">
-        <v>1.30634</v>
+        <v>1.31339</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>43390</v>
+        <v>43392</v>
       </c>
       <c r="B40">
-        <v>-0.9999999999998899</v>
+        <v>-3</v>
       </c>
       <c r="C40">
-        <v>1.31349</v>
+        <v>1.30471</v>
       </c>
       <c r="D40">
-        <v>1.31339</v>
+        <v>1.30441</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>43392</v>
+        <v>43395</v>
       </c>
       <c r="B41">
-        <v>-2.99999999999967</v>
+        <v>-1.6</v>
       </c>
       <c r="C41">
-        <v>1.30471</v>
+        <v>1.2974</v>
       </c>
       <c r="D41">
-        <v>1.30441</v>
+        <v>1.29724</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>43395</v>
+        <v>43410</v>
       </c>
       <c r="B42">
-        <v>-1.6000000000016</v>
+        <v>-0.7</v>
       </c>
       <c r="C42">
-        <v>1.2974</v>
+        <v>1.30781</v>
       </c>
       <c r="D42">
-        <v>1.29724</v>
+        <v>1.30774</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>43410</v>
+        <v>43451</v>
       </c>
       <c r="B43">
-        <v>-0.7000000000023654</v>
+        <v>-1.6</v>
       </c>
       <c r="C43">
-        <v>1.30781</v>
+        <v>1.26081</v>
       </c>
       <c r="D43">
-        <v>1.30774</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2">
-        <v>43451</v>
-      </c>
-      <c r="B44">
-        <v>-1.59999999999938</v>
-      </c>
-      <c r="C44">
-        <v>1.26081</v>
-      </c>
-      <c r="D44">
         <v>1.26065</v>
       </c>
     </row>
@@ -5576,7 +5520,7 @@
         <v>43104</v>
       </c>
       <c r="B2">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C2">
         <v>1.35534</v>
@@ -5590,7 +5534,7 @@
         <v>43110</v>
       </c>
       <c r="B3">
-        <v>-3.60000000000138</v>
+        <v>-3.6</v>
       </c>
       <c r="C3">
         <v>1.35315</v>
@@ -5604,7 +5548,7 @@
         <v>43123</v>
       </c>
       <c r="B4">
-        <v>-0.5999999999972694</v>
+        <v>-0.6</v>
       </c>
       <c r="C4">
         <v>1.40138</v>
@@ -5618,7 +5562,7 @@
         <v>43133</v>
       </c>
       <c r="B5">
-        <v>-2.900000000001235</v>
+        <v>-2.9</v>
       </c>
       <c r="C5">
         <v>1.41291</v>
@@ -5632,7 +5576,7 @@
         <v>43136</v>
       </c>
       <c r="B6">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C6">
         <v>1.40236</v>
@@ -5646,7 +5590,7 @@
         <v>43143</v>
       </c>
       <c r="B7">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C7">
         <v>1.38067</v>
@@ -5660,7 +5604,7 @@
         <v>43146</v>
       </c>
       <c r="B8">
-        <v>-5.300000000001415</v>
+        <v>-5.3</v>
       </c>
       <c r="C8">
         <v>1.40657</v>
@@ -5674,7 +5618,7 @@
         <v>43147</v>
       </c>
       <c r="B9">
-        <v>-3.199999999998759</v>
+        <v>-3.2</v>
       </c>
       <c r="C9">
         <v>1.40462</v>
@@ -5688,7 +5632,7 @@
         <v>43153</v>
       </c>
       <c r="B10">
-        <v>-1.699999999997814</v>
+        <v>-1.7</v>
       </c>
       <c r="C10">
         <v>1.39413</v>
@@ -5702,7 +5646,7 @@
         <v>43161</v>
       </c>
       <c r="B11">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C11">
         <v>1.37769</v>
@@ -5716,7 +5660,7 @@
         <v>43165</v>
       </c>
       <c r="B12">
-        <v>-2.80000000000058</v>
+        <v>-2.8</v>
       </c>
       <c r="C12">
         <v>1.38924</v>
@@ -5730,7 +5674,7 @@
         <v>43180</v>
       </c>
       <c r="B13">
-        <v>-1.399999999998069</v>
+        <v>-1.4</v>
       </c>
       <c r="C13">
         <v>1.40705</v>
@@ -5744,7 +5688,7 @@
         <v>43189</v>
       </c>
       <c r="B14">
-        <v>-2.500000000000835</v>
+        <v>-2.5</v>
       </c>
       <c r="C14">
         <v>1.40365</v>
@@ -5758,7 +5702,7 @@
         <v>43192</v>
       </c>
       <c r="B15">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C15">
         <v>1.40542</v>
@@ -5772,7 +5716,7 @@
         <v>43194</v>
       </c>
       <c r="B16">
-        <v>-3.999999999999559</v>
+        <v>-4</v>
       </c>
       <c r="C16">
         <v>1.40841</v>
@@ -5786,7 +5730,7 @@
         <v>43200</v>
       </c>
       <c r="B17">
-        <v>-5.299999999999194</v>
+        <v>-5.3</v>
       </c>
       <c r="C17">
         <v>1.41759</v>
@@ -5800,7 +5744,7 @@
         <v>43201</v>
       </c>
       <c r="B18">
-        <v>-1.500000000000945</v>
+        <v>-1.5</v>
       </c>
       <c r="C18">
         <v>1.42048</v>
@@ -5814,7 +5758,7 @@
         <v>43207</v>
       </c>
       <c r="B19">
-        <v>-1.899999999999125</v>
+        <v>-1.9</v>
       </c>
       <c r="C19">
         <v>1.43095</v>
@@ -5828,7 +5772,7 @@
         <v>43214</v>
       </c>
       <c r="B20">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C20">
         <v>1.39644</v>
@@ -5842,7 +5786,7 @@
         <v>43220</v>
       </c>
       <c r="B21">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C21">
         <v>1.37687</v>
@@ -5856,7 +5800,7 @@
         <v>43230</v>
       </c>
       <c r="B22">
-        <v>-3.899999999998904</v>
+        <v>-3.9</v>
       </c>
       <c r="C22">
         <v>1.34723</v>
@@ -5870,7 +5814,7 @@
         <v>43236</v>
       </c>
       <c r="B23">
-        <v>-4.100000000000215</v>
+        <v>-4.1</v>
       </c>
       <c r="C23">
         <v>1.34873</v>
@@ -5884,7 +5828,7 @@
         <v>43248</v>
       </c>
       <c r="B24">
-        <v>-5.100000000000104</v>
+        <v>-5.1</v>
       </c>
       <c r="C24">
         <v>1.33045</v>
@@ -5898,7 +5842,7 @@
         <v>43257</v>
       </c>
       <c r="B25">
-        <v>-2.19999999999887</v>
+        <v>-2.2</v>
       </c>
       <c r="C25">
         <v>1.34273</v>
@@ -5912,7 +5856,7 @@
         <v>43262</v>
       </c>
       <c r="B26">
-        <v>-3.599999999999159</v>
+        <v>-3.6</v>
       </c>
       <c r="C26">
         <v>1.33961</v>
@@ -5926,7 +5870,7 @@
         <v>43276</v>
       </c>
       <c r="B27">
-        <v>-5.899999999998684</v>
+        <v>-5.9</v>
       </c>
       <c r="C27">
         <v>1.3272</v>
@@ -5940,7 +5884,7 @@
         <v>43284</v>
       </c>
       <c r="B28">
-        <v>-0.7999999999985796</v>
+        <v>-0.8</v>
       </c>
       <c r="C28">
         <v>1.3173</v>
@@ -5954,7 +5898,7 @@
         <v>43286</v>
       </c>
       <c r="B29">
-        <v>-4.300000000001525</v>
+        <v>-4.3</v>
       </c>
       <c r="C29">
         <v>1.32247</v>
@@ -5968,7 +5912,7 @@
         <v>43287</v>
       </c>
       <c r="B30">
-        <v>-0.4000000000004</v>
+        <v>-0.4</v>
       </c>
       <c r="C30">
         <v>1.32713</v>
@@ -5982,7 +5926,7 @@
         <v>43311</v>
       </c>
       <c r="B31">
-        <v>-3.599999999996939</v>
+        <v>-3.6</v>
       </c>
       <c r="C31">
         <v>1.31488</v>
@@ -5996,7 +5940,7 @@
         <v>43313</v>
       </c>
       <c r="B32">
-        <v>-2.99999999999967</v>
+        <v>-3</v>
       </c>
       <c r="C32">
         <v>1.31248</v>
@@ -6010,7 +5954,7 @@
         <v>43328</v>
       </c>
       <c r="B33">
-        <v>-1.100000000000545</v>
+        <v>-1.1</v>
       </c>
       <c r="C33">
         <v>1.27291</v>
@@ -6024,7 +5968,7 @@
         <v>43333</v>
       </c>
       <c r="B34">
-        <v>-3.20000000000098</v>
+        <v>-3.2</v>
       </c>
       <c r="C34">
         <v>1.28678</v>
@@ -6038,7 +5982,7 @@
         <v>43334</v>
       </c>
       <c r="B35">
-        <v>-4.299999999999304</v>
+        <v>-4.3</v>
       </c>
       <c r="C35">
         <v>1.29129</v>
@@ -6052,7 +5996,7 @@
         <v>43335</v>
       </c>
       <c r="B36">
-        <v>-4.599999999999049</v>
+        <v>-4.6</v>
       </c>
       <c r="C36">
         <v>1.28388</v>
@@ -6066,7 +6010,7 @@
         <v>43340</v>
       </c>
       <c r="B37">
-        <v>-1.99999999999978</v>
+        <v>-2</v>
       </c>
       <c r="C37">
         <v>1.28838</v>
@@ -6080,7 +6024,7 @@
         <v>43353</v>
       </c>
       <c r="B38">
-        <v>-4.499999999998394</v>
+        <v>-4.5</v>
       </c>
       <c r="C38">
         <v>1.30257</v>
@@ -6094,7 +6038,7 @@
         <v>43355</v>
       </c>
       <c r="B39">
-        <v>-0.4000000000026205</v>
+        <v>-0.4</v>
       </c>
       <c r="C39">
         <v>1.30212</v>
@@ -6108,7 +6052,7 @@
         <v>43357</v>
       </c>
       <c r="B40">
-        <v>-4.699999999999704</v>
+        <v>-4.7</v>
       </c>
       <c r="C40">
         <v>1.30782</v>
@@ -6122,7 +6066,7 @@
         <v>43361</v>
       </c>
       <c r="B41">
-        <v>-2.60000000000149</v>
+        <v>-2.6</v>
       </c>
       <c r="C41">
         <v>1.31535</v>
@@ -6136,7 +6080,7 @@
         <v>43377</v>
       </c>
       <c r="B42">
-        <v>-4.900000000001015</v>
+        <v>-4.9</v>
       </c>
       <c r="C42">
         <v>1.30328</v>
@@ -6150,7 +6094,7 @@
         <v>43381</v>
       </c>
       <c r="B43">
-        <v>-4.999999999999449</v>
+        <v>-5</v>
       </c>
       <c r="C43">
         <v>1.30684</v>
@@ -6164,7 +6108,7 @@
         <v>43390</v>
       </c>
       <c r="B44">
-        <v>-0.9999999999998899</v>
+        <v>-1</v>
       </c>
       <c r="C44">
         <v>1.31349</v>
@@ -6178,7 +6122,7 @@
         <v>43392</v>
       </c>
       <c r="B45">
-        <v>-2.99999999999967</v>
+        <v>-3</v>
       </c>
       <c r="C45">
         <v>1.30471</v>
@@ -6192,7 +6136,7 @@
         <v>43395</v>
       </c>
       <c r="B46">
-        <v>-1.6000000000016</v>
+        <v>-1.6</v>
       </c>
       <c r="C46">
         <v>1.2974</v>
@@ -6206,7 +6150,7 @@
         <v>43410</v>
       </c>
       <c r="B47">
-        <v>-0.7000000000023654</v>
+        <v>-0.7</v>
       </c>
       <c r="C47">
         <v>1.30781</v>
@@ -6220,7 +6164,7 @@
         <v>43424</v>
       </c>
       <c r="B48">
-        <v>-5.500000000000504</v>
+        <v>-5.5</v>
       </c>
       <c r="C48">
         <v>1.28275</v>
@@ -6234,7 +6178,7 @@
         <v>43451</v>
       </c>
       <c r="B49">
-        <v>-1.59999999999938</v>
+        <v>-1.6</v>
       </c>
       <c r="C49">
         <v>1.26081</v>
@@ -6248,7 +6192,7 @@
         <v>43454</v>
       </c>
       <c r="B50">
-        <v>-5.699999999999594</v>
+        <v>-5.7</v>
       </c>
       <c r="C50">
         <v>1.26416</v>

</xml_diff>